<commit_message>
Successful generation of basic train and personnel schedules -Schedules displayed successfully in GUI
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,81 @@
   </si>
   <si>
     <t>Departure</t>
+  </si>
+  <si>
+    <t>SHADYSIDE</t>
+  </si>
+  <si>
+    <t>HERRON</t>
+  </si>
+  <si>
+    <t>SWISSVILLE</t>
+  </si>
+  <si>
+    <t>PENN STATION</t>
+  </si>
+  <si>
+    <t>STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>FIRST AVE</t>
+  </si>
+  <si>
+    <t>ST SQUARE</t>
+  </si>
+  <si>
+    <t>STH HILLS</t>
+  </si>
+  <si>
+    <t>Employee 1</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>2pm - 10:30pm</t>
+  </si>
+  <si>
+    <t>6.7.0</t>
+  </si>
+  <si>
+    <t>Employee 2</t>
+  </si>
+  <si>
+    <t>6am - 2:30pm</t>
+  </si>
+  <si>
+    <t>6.14.0</t>
+  </si>
+  <si>
+    <t>Employee 3</t>
+  </si>
+  <si>
+    <t>6.21.0</t>
+  </si>
+  <si>
+    <t>Employee 4</t>
+  </si>
+  <si>
+    <t>6.28.0</t>
+  </si>
+  <si>
+    <t>Employee 5</t>
+  </si>
+  <si>
+    <t>6.35.0</t>
+  </si>
+  <si>
+    <t>Employee 6</t>
+  </si>
+  <si>
+    <t>6.42.0</t>
+  </si>
+  <si>
+    <t>Employee 7</t>
+  </si>
+  <si>
+    <t>6.49.0</t>
   </si>
 </sst>
 </file>
@@ -123,6 +198,188 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -146,6 +403,107 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -170,7 +528,38 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Schedule generation now creates slightly better schedules
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -82,46 +82,43 @@
     <t>2pm - 10:30pm</t>
   </si>
   <si>
+    <t>Employee 2</t>
+  </si>
+  <si>
+    <t>6am - 2:30pm</t>
+  </si>
+  <si>
+    <t>06.00.00</t>
+  </si>
+  <si>
+    <t>Employee 3</t>
+  </si>
+  <si>
+    <t>14.00.00</t>
+  </si>
+  <si>
+    <t>Employee 4</t>
+  </si>
+  <si>
     <t>6.7.0</t>
   </si>
   <si>
-    <t>Employee 2</t>
-  </si>
-  <si>
-    <t>6am - 2:30pm</t>
+    <t>Employee 5</t>
+  </si>
+  <si>
+    <t>2.7.0</t>
+  </si>
+  <si>
+    <t>Employee 6</t>
   </si>
   <si>
     <t>6.14.0</t>
   </si>
   <si>
-    <t>Employee 3</t>
-  </si>
-  <si>
-    <t>6.21.0</t>
-  </si>
-  <si>
-    <t>Employee 4</t>
-  </si>
-  <si>
-    <t>6.28.0</t>
-  </si>
-  <si>
-    <t>Employee 5</t>
-  </si>
-  <si>
-    <t>6.35.0</t>
-  </si>
-  <si>
-    <t>Employee 6</t>
-  </si>
-  <si>
-    <t>6.42.0</t>
-  </si>
-  <si>
     <t>Employee 7</t>
   </si>
   <si>
-    <t>6.49.0</t>
+    <t>2.14.0</t>
   </si>
 </sst>
 </file>
@@ -226,10 +223,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -238,21 +235,21 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -278,16 +275,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>20</v>
@@ -296,15 +293,15 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -330,22 +327,22 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
@@ -356,7 +353,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -428,26 +425,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>101.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="3">
       <c r="A3" t="n">
         <v>102.0</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -455,10 +441,10 @@
         <v>103.0</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -466,10 +452,10 @@
         <v>104.0</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6">
@@ -477,10 +463,10 @@
         <v>105.0</v>
       </c>
       <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7">
@@ -488,10 +474,10 @@
         <v>106.0</v>
       </c>
       <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8">
@@ -499,10 +485,10 @@
         <v>107.0</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an issue where certain scheduled times were displaying "AM" instead of "PM"
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="115">
   <si>
     <t>Name</t>
   </si>
@@ -119,6 +119,246 @@
   </si>
   <si>
     <t>2.14.0</t>
+  </si>
+  <si>
+    <t>Employee 8</t>
+  </si>
+  <si>
+    <t>6.21.0</t>
+  </si>
+  <si>
+    <t>Employee 9</t>
+  </si>
+  <si>
+    <t>Employee 10</t>
+  </si>
+  <si>
+    <t>6.28.0</t>
+  </si>
+  <si>
+    <t>Employee 11</t>
+  </si>
+  <si>
+    <t>2.21.0</t>
+  </si>
+  <si>
+    <t>Employee 12</t>
+  </si>
+  <si>
+    <t>6.35.0</t>
+  </si>
+  <si>
+    <t>Employee 13</t>
+  </si>
+  <si>
+    <t>2.28.0</t>
+  </si>
+  <si>
+    <t>Employee 14</t>
+  </si>
+  <si>
+    <t>6.42.0</t>
+  </si>
+  <si>
+    <t>Employee 15</t>
+  </si>
+  <si>
+    <t>2.35.0</t>
+  </si>
+  <si>
+    <t>Employee 16</t>
+  </si>
+  <si>
+    <t>6.49.0</t>
+  </si>
+  <si>
+    <t>Employee 17</t>
+  </si>
+  <si>
+    <t>Employee 18</t>
+  </si>
+  <si>
+    <t>6.56.0</t>
+  </si>
+  <si>
+    <t>Employee 19</t>
+  </si>
+  <si>
+    <t>2.42.0</t>
+  </si>
+  <si>
+    <t>Employee 20</t>
+  </si>
+  <si>
+    <t>7.3.0</t>
+  </si>
+  <si>
+    <t>Employee 21</t>
+  </si>
+  <si>
+    <t>2.49.0</t>
+  </si>
+  <si>
+    <t>Employee 22</t>
+  </si>
+  <si>
+    <t>7.10.0</t>
+  </si>
+  <si>
+    <t>Employee 23</t>
+  </si>
+  <si>
+    <t>2.56.0</t>
+  </si>
+  <si>
+    <t>Employee 24</t>
+  </si>
+  <si>
+    <t>7.17.0</t>
+  </si>
+  <si>
+    <t>Employee 25</t>
+  </si>
+  <si>
+    <t>Employee 26</t>
+  </si>
+  <si>
+    <t>7.24.0</t>
+  </si>
+  <si>
+    <t>Employee 27</t>
+  </si>
+  <si>
+    <t>3.3.0</t>
+  </si>
+  <si>
+    <t>Employee 28</t>
+  </si>
+  <si>
+    <t>7.31.0</t>
+  </si>
+  <si>
+    <t>Employee 29</t>
+  </si>
+  <si>
+    <t>3.10.0</t>
+  </si>
+  <si>
+    <t>Employee 30</t>
+  </si>
+  <si>
+    <t>7.38.0</t>
+  </si>
+  <si>
+    <t>Employee 31</t>
+  </si>
+  <si>
+    <t>3.17.0</t>
+  </si>
+  <si>
+    <t>Employee 32</t>
+  </si>
+  <si>
+    <t>7.45.0</t>
+  </si>
+  <si>
+    <t>Employee 33</t>
+  </si>
+  <si>
+    <t>Employee 34</t>
+  </si>
+  <si>
+    <t>7.52.0</t>
+  </si>
+  <si>
+    <t>Employee 35</t>
+  </si>
+  <si>
+    <t>3.24.0</t>
+  </si>
+  <si>
+    <t>Employee 36</t>
+  </si>
+  <si>
+    <t>7.59.0</t>
+  </si>
+  <si>
+    <t>Employee 37</t>
+  </si>
+  <si>
+    <t>3.31.0</t>
+  </si>
+  <si>
+    <t>Employee 38</t>
+  </si>
+  <si>
+    <t>8.6.0</t>
+  </si>
+  <si>
+    <t>Employee 39</t>
+  </si>
+  <si>
+    <t>3.38.0</t>
+  </si>
+  <si>
+    <t>Employee 40</t>
+  </si>
+  <si>
+    <t>8.13.0</t>
+  </si>
+  <si>
+    <t>Employee 41</t>
+  </si>
+  <si>
+    <t>Employee 42</t>
+  </si>
+  <si>
+    <t>8.20.0</t>
+  </si>
+  <si>
+    <t>Employee 43</t>
+  </si>
+  <si>
+    <t>3.45.0</t>
+  </si>
+  <si>
+    <t>Employee 44</t>
+  </si>
+  <si>
+    <t>8.27.0</t>
+  </si>
+  <si>
+    <t>Employee 45</t>
+  </si>
+  <si>
+    <t>3.52.0</t>
+  </si>
+  <si>
+    <t>Employee 46</t>
+  </si>
+  <si>
+    <t>8.34.0</t>
+  </si>
+  <si>
+    <t>Employee 47</t>
+  </si>
+  <si>
+    <t>3.59.0</t>
+  </si>
+  <si>
+    <t>Employee 48</t>
+  </si>
+  <si>
+    <t>8.41.0</t>
+  </si>
+  <si>
+    <t>Employee 49</t>
+  </si>
+  <si>
+    <t>Employee 50</t>
+  </si>
+  <si>
+    <t>8.48.0</t>
   </si>
 </sst>
 </file>
@@ -377,6 +617,1124 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" t="s">
+        <v>23</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" t="s">
+        <v>23</v>
+      </c>
+      <c r="H51" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -491,6 +1849,413 @@
         <v>34</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>119.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>131.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>134.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>135.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>136.0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>137.0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>139.0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>140.0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>142.0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>143.0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>145.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>146.0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>147.0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>148.0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -546,6 +2311,49 @@
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Train Handler updated to dispatch new trains and update all the trains currently on the track
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="269">
   <si>
     <t>Name</t>
   </si>
@@ -359,6 +359,468 @@
   </si>
   <si>
     <t>8.48.0</t>
+  </si>
+  <si>
+    <t>Employee 51</t>
+  </si>
+  <si>
+    <t>4.6.0</t>
+  </si>
+  <si>
+    <t>Employee 52</t>
+  </si>
+  <si>
+    <t>8.55.0</t>
+  </si>
+  <si>
+    <t>Employee 53</t>
+  </si>
+  <si>
+    <t>4.13.0</t>
+  </si>
+  <si>
+    <t>Employee 54</t>
+  </si>
+  <si>
+    <t>9.2.0</t>
+  </si>
+  <si>
+    <t>Employee 55</t>
+  </si>
+  <si>
+    <t>4.20.0</t>
+  </si>
+  <si>
+    <t>Employee 56</t>
+  </si>
+  <si>
+    <t>9.9.0</t>
+  </si>
+  <si>
+    <t>Employee 57</t>
+  </si>
+  <si>
+    <t>Employee 58</t>
+  </si>
+  <si>
+    <t>9.16.0</t>
+  </si>
+  <si>
+    <t>Employee 59</t>
+  </si>
+  <si>
+    <t>4.27.0</t>
+  </si>
+  <si>
+    <t>Employee 60</t>
+  </si>
+  <si>
+    <t>9.23.0</t>
+  </si>
+  <si>
+    <t>Employee 61</t>
+  </si>
+  <si>
+    <t>4.34.0</t>
+  </si>
+  <si>
+    <t>Employee 62</t>
+  </si>
+  <si>
+    <t>9.30.0</t>
+  </si>
+  <si>
+    <t>Employee 63</t>
+  </si>
+  <si>
+    <t>4.41.0</t>
+  </si>
+  <si>
+    <t>Employee 64</t>
+  </si>
+  <si>
+    <t>9.37.0</t>
+  </si>
+  <si>
+    <t>Employee 65</t>
+  </si>
+  <si>
+    <t>Employee 66</t>
+  </si>
+  <si>
+    <t>9.44.0</t>
+  </si>
+  <si>
+    <t>Employee 67</t>
+  </si>
+  <si>
+    <t>4.48.0</t>
+  </si>
+  <si>
+    <t>Employee 68</t>
+  </si>
+  <si>
+    <t>9.51.0</t>
+  </si>
+  <si>
+    <t>Employee 69</t>
+  </si>
+  <si>
+    <t>4.55.0</t>
+  </si>
+  <si>
+    <t>Employee 70</t>
+  </si>
+  <si>
+    <t>9.58.0</t>
+  </si>
+  <si>
+    <t>Employee 71</t>
+  </si>
+  <si>
+    <t>5.2.0</t>
+  </si>
+  <si>
+    <t>Employee 72</t>
+  </si>
+  <si>
+    <t>10.5.0</t>
+  </si>
+  <si>
+    <t>Employee 73</t>
+  </si>
+  <si>
+    <t>Employee 74</t>
+  </si>
+  <si>
+    <t>10.12.0</t>
+  </si>
+  <si>
+    <t>Employee 75</t>
+  </si>
+  <si>
+    <t>5.9.0</t>
+  </si>
+  <si>
+    <t>Employee 76</t>
+  </si>
+  <si>
+    <t>10.19.0</t>
+  </si>
+  <si>
+    <t>Employee 77</t>
+  </si>
+  <si>
+    <t>5.16.0</t>
+  </si>
+  <si>
+    <t>Employee 78</t>
+  </si>
+  <si>
+    <t>10.26.0</t>
+  </si>
+  <si>
+    <t>Employee 79</t>
+  </si>
+  <si>
+    <t>5.23.0</t>
+  </si>
+  <si>
+    <t>Employee 80</t>
+  </si>
+  <si>
+    <t>10.33.0</t>
+  </si>
+  <si>
+    <t>Employee 81</t>
+  </si>
+  <si>
+    <t>Employee 82</t>
+  </si>
+  <si>
+    <t>10.40.0</t>
+  </si>
+  <si>
+    <t>Employee 83</t>
+  </si>
+  <si>
+    <t>5.30.0</t>
+  </si>
+  <si>
+    <t>Employee 84</t>
+  </si>
+  <si>
+    <t>10.47.0</t>
+  </si>
+  <si>
+    <t>Employee 85</t>
+  </si>
+  <si>
+    <t>5.37.0</t>
+  </si>
+  <si>
+    <t>Employee 86</t>
+  </si>
+  <si>
+    <t>10.54.0</t>
+  </si>
+  <si>
+    <t>Employee 87</t>
+  </si>
+  <si>
+    <t>5.44.0</t>
+  </si>
+  <si>
+    <t>Employee 88</t>
+  </si>
+  <si>
+    <t>11.1.0</t>
+  </si>
+  <si>
+    <t>Employee 89</t>
+  </si>
+  <si>
+    <t>Employee 90</t>
+  </si>
+  <si>
+    <t>11.8.0</t>
+  </si>
+  <si>
+    <t>Employee 91</t>
+  </si>
+  <si>
+    <t>5.51.0</t>
+  </si>
+  <si>
+    <t>Employee 92</t>
+  </si>
+  <si>
+    <t>11.15.0</t>
+  </si>
+  <si>
+    <t>Employee 93</t>
+  </si>
+  <si>
+    <t>5.58.0</t>
+  </si>
+  <si>
+    <t>Employee 94</t>
+  </si>
+  <si>
+    <t>11.22.0</t>
+  </si>
+  <si>
+    <t>Employee 95</t>
+  </si>
+  <si>
+    <t>6.5.0</t>
+  </si>
+  <si>
+    <t>Employee 96</t>
+  </si>
+  <si>
+    <t>11.29.0</t>
+  </si>
+  <si>
+    <t>Employee 97</t>
+  </si>
+  <si>
+    <t>Employee 98</t>
+  </si>
+  <si>
+    <t>11.36.0</t>
+  </si>
+  <si>
+    <t>Employee 99</t>
+  </si>
+  <si>
+    <t>6.12.0</t>
+  </si>
+  <si>
+    <t>Employee 100</t>
+  </si>
+  <si>
+    <t>11.43.0</t>
+  </si>
+  <si>
+    <t>Employee 101</t>
+  </si>
+  <si>
+    <t>6.19.0</t>
+  </si>
+  <si>
+    <t>Employee 102</t>
+  </si>
+  <si>
+    <t>11.50.0</t>
+  </si>
+  <si>
+    <t>Employee 103</t>
+  </si>
+  <si>
+    <t>6.26.0</t>
+  </si>
+  <si>
+    <t>Employee 104</t>
+  </si>
+  <si>
+    <t>11.57.0</t>
+  </si>
+  <si>
+    <t>Employee 105</t>
+  </si>
+  <si>
+    <t>Employee 106</t>
+  </si>
+  <si>
+    <t>12.4.0</t>
+  </si>
+  <si>
+    <t>Employee 107</t>
+  </si>
+  <si>
+    <t>6.33.0</t>
+  </si>
+  <si>
+    <t>Employee 108</t>
+  </si>
+  <si>
+    <t>12.11.0</t>
+  </si>
+  <si>
+    <t>Employee 109</t>
+  </si>
+  <si>
+    <t>6.40.0</t>
+  </si>
+  <si>
+    <t>Employee 110</t>
+  </si>
+  <si>
+    <t>12.18.0</t>
+  </si>
+  <si>
+    <t>Employee 111</t>
+  </si>
+  <si>
+    <t>6.47.0</t>
+  </si>
+  <si>
+    <t>Employee 112</t>
+  </si>
+  <si>
+    <t>12.25.0</t>
+  </si>
+  <si>
+    <t>Employee 113</t>
+  </si>
+  <si>
+    <t>Employee 114</t>
+  </si>
+  <si>
+    <t>12.32.0</t>
+  </si>
+  <si>
+    <t>Employee 115</t>
+  </si>
+  <si>
+    <t>6.54.0</t>
+  </si>
+  <si>
+    <t>Employee 116</t>
+  </si>
+  <si>
+    <t>12.39.0</t>
+  </si>
+  <si>
+    <t>Employee 117</t>
+  </si>
+  <si>
+    <t>7.1.0</t>
+  </si>
+  <si>
+    <t>Employee 118</t>
+  </si>
+  <si>
+    <t>12.46.0</t>
+  </si>
+  <si>
+    <t>Employee 119</t>
+  </si>
+  <si>
+    <t>7.8.0</t>
+  </si>
+  <si>
+    <t>Employee 120</t>
+  </si>
+  <si>
+    <t>12.53.0</t>
+  </si>
+  <si>
+    <t>Employee 121</t>
+  </si>
+  <si>
+    <t>Employee 122</t>
+  </si>
+  <si>
+    <t>12.60.0</t>
+  </si>
+  <si>
+    <t>Employee 123</t>
+  </si>
+  <si>
+    <t>7.15.0</t>
+  </si>
+  <si>
+    <t>Employee 124</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
+  </si>
+  <si>
+    <t>Employee 125</t>
+  </si>
+  <si>
+    <t>7.22.0</t>
+  </si>
+  <si>
+    <t>Employee 126</t>
+  </si>
+  <si>
+    <t>1.14.0</t>
+  </si>
+  <si>
+    <t>Employee 127</t>
+  </si>
+  <si>
+    <t>7.29.0</t>
+  </si>
+  <si>
+    <t>Employee 128</t>
+  </si>
+  <si>
+    <t>1.21.0</t>
+  </si>
+  <si>
+    <t>Employee 129</t>
+  </si>
+  <si>
+    <t>Employee 130</t>
+  </si>
+  <si>
+    <t>1.28.0</t>
+  </si>
+  <si>
+    <t>Employee 131</t>
+  </si>
+  <si>
+    <t>7.36.0</t>
+  </si>
+  <si>
+    <t>Employee 132</t>
+  </si>
+  <si>
+    <t>1.35.0</t>
   </si>
 </sst>
 </file>
@@ -1735,6 +2197,2138 @@
         <v>23</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>115</v>
+      </c>
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C54" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" t="s">
+        <v>23</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" t="s">
+        <v>21</v>
+      </c>
+      <c r="G56" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="D57" t="s">
+        <v>23</v>
+      </c>
+      <c r="E57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" t="s">
+        <v>23</v>
+      </c>
+      <c r="H57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" t="s">
+        <v>21</v>
+      </c>
+      <c r="G58" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>20</v>
+      </c>
+      <c r="E59" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>23</v>
+      </c>
+      <c r="H59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" t="s">
+        <v>23</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" t="s">
+        <v>23</v>
+      </c>
+      <c r="E61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" t="s">
+        <v>23</v>
+      </c>
+      <c r="H61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B62" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" t="s">
+        <v>21</v>
+      </c>
+      <c r="F62" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="D63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>21</v>
+      </c>
+      <c r="D64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" t="s">
+        <v>21</v>
+      </c>
+      <c r="F64" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" t="s">
+        <v>21</v>
+      </c>
+      <c r="H64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>140</v>
+      </c>
+      <c r="B65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" t="s">
+        <v>23</v>
+      </c>
+      <c r="E65" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>23</v>
+      </c>
+      <c r="H65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>142</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" t="s">
+        <v>21</v>
+      </c>
+      <c r="F66" t="s">
+        <v>21</v>
+      </c>
+      <c r="G66" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B67" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" t="s">
+        <v>23</v>
+      </c>
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>23</v>
+      </c>
+      <c r="H67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" t="s">
+        <v>21</v>
+      </c>
+      <c r="H68" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" t="s">
+        <v>21</v>
+      </c>
+      <c r="F70" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>151</v>
+      </c>
+      <c r="B71" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>23</v>
+      </c>
+      <c r="E71" t="s">
+        <v>23</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" t="s">
+        <v>21</v>
+      </c>
+      <c r="C72" t="s">
+        <v>21</v>
+      </c>
+      <c r="D72" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" t="s">
+        <v>21</v>
+      </c>
+      <c r="F72" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" t="s">
+        <v>21</v>
+      </c>
+      <c r="H72" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>155</v>
+      </c>
+      <c r="B73" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" t="s">
+        <v>23</v>
+      </c>
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" t="s">
+        <v>23</v>
+      </c>
+      <c r="H73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" t="s">
+        <v>20</v>
+      </c>
+      <c r="D74" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" t="s">
+        <v>21</v>
+      </c>
+      <c r="G74" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>158</v>
+      </c>
+      <c r="B75" t="s">
+        <v>23</v>
+      </c>
+      <c r="C75" t="s">
+        <v>20</v>
+      </c>
+      <c r="D75" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" t="s">
+        <v>23</v>
+      </c>
+      <c r="G75" t="s">
+        <v>23</v>
+      </c>
+      <c r="H75" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>160</v>
+      </c>
+      <c r="B76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" t="s">
+        <v>21</v>
+      </c>
+      <c r="G76" t="s">
+        <v>21</v>
+      </c>
+      <c r="H76" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>162</v>
+      </c>
+      <c r="B77" t="s">
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77" t="s">
+        <v>20</v>
+      </c>
+      <c r="G77" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>164</v>
+      </c>
+      <c r="B78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C78" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" t="s">
+        <v>20</v>
+      </c>
+      <c r="G78" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>166</v>
+      </c>
+      <c r="B79" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" t="s">
+        <v>23</v>
+      </c>
+      <c r="F79" t="s">
+        <v>23</v>
+      </c>
+      <c r="G79" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>168</v>
+      </c>
+      <c r="B80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" t="s">
+        <v>21</v>
+      </c>
+      <c r="G80" t="s">
+        <v>21</v>
+      </c>
+      <c r="H80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>170</v>
+      </c>
+      <c r="B81" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E81" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" t="s">
+        <v>23</v>
+      </c>
+      <c r="H81" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>172</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>20</v>
+      </c>
+      <c r="D82" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" t="s">
+        <v>21</v>
+      </c>
+      <c r="F82" t="s">
+        <v>21</v>
+      </c>
+      <c r="G82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H82" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B83" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" t="s">
+        <v>20</v>
+      </c>
+      <c r="D83" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" t="s">
+        <v>23</v>
+      </c>
+      <c r="F83" t="s">
+        <v>23</v>
+      </c>
+      <c r="G83" t="s">
+        <v>23</v>
+      </c>
+      <c r="H83" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" t="s">
+        <v>21</v>
+      </c>
+      <c r="C84" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" t="s">
+        <v>20</v>
+      </c>
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84" t="s">
+        <v>21</v>
+      </c>
+      <c r="G84" t="s">
+        <v>21</v>
+      </c>
+      <c r="H84" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>177</v>
+      </c>
+      <c r="B85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85" t="s">
+        <v>20</v>
+      </c>
+      <c r="G85" t="s">
+        <v>23</v>
+      </c>
+      <c r="H85" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>179</v>
+      </c>
+      <c r="B86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" t="s">
+        <v>21</v>
+      </c>
+      <c r="D86" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" t="s">
+        <v>20</v>
+      </c>
+      <c r="G86" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>181</v>
+      </c>
+      <c r="B87" t="s">
+        <v>23</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E87" t="s">
+        <v>23</v>
+      </c>
+      <c r="F87" t="s">
+        <v>23</v>
+      </c>
+      <c r="G87" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>183</v>
+      </c>
+      <c r="B88" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" t="s">
+        <v>21</v>
+      </c>
+      <c r="D88" t="s">
+        <v>21</v>
+      </c>
+      <c r="E88" t="s">
+        <v>21</v>
+      </c>
+      <c r="F88" t="s">
+        <v>21</v>
+      </c>
+      <c r="G88" t="s">
+        <v>21</v>
+      </c>
+      <c r="H88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>185</v>
+      </c>
+      <c r="B89" t="s">
+        <v>23</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>23</v>
+      </c>
+      <c r="H89" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>187</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" t="s">
+        <v>21</v>
+      </c>
+      <c r="F90" t="s">
+        <v>21</v>
+      </c>
+      <c r="G90" t="s">
+        <v>21</v>
+      </c>
+      <c r="H90" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>188</v>
+      </c>
+      <c r="B91" t="s">
+        <v>23</v>
+      </c>
+      <c r="C91" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" t="s">
+        <v>20</v>
+      </c>
+      <c r="E91" t="s">
+        <v>23</v>
+      </c>
+      <c r="F91" t="s">
+        <v>23</v>
+      </c>
+      <c r="G91" t="s">
+        <v>23</v>
+      </c>
+      <c r="H91" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>190</v>
+      </c>
+      <c r="B92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" t="s">
+        <v>21</v>
+      </c>
+      <c r="D92" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
+        <v>21</v>
+      </c>
+      <c r="G92" t="s">
+        <v>21</v>
+      </c>
+      <c r="H92" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>192</v>
+      </c>
+      <c r="B93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C93" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F93" t="s">
+        <v>20</v>
+      </c>
+      <c r="G93" t="s">
+        <v>23</v>
+      </c>
+      <c r="H93" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>194</v>
+      </c>
+      <c r="B94" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" t="s">
+        <v>21</v>
+      </c>
+      <c r="D94" t="s">
+        <v>21</v>
+      </c>
+      <c r="E94" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" t="s">
+        <v>20</v>
+      </c>
+      <c r="G94" t="s">
+        <v>20</v>
+      </c>
+      <c r="H94" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>196</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" t="s">
+        <v>23</v>
+      </c>
+      <c r="E95" t="s">
+        <v>23</v>
+      </c>
+      <c r="F95" t="s">
+        <v>23</v>
+      </c>
+      <c r="G95" t="s">
+        <v>20</v>
+      </c>
+      <c r="H95" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>198</v>
+      </c>
+      <c r="B96" t="s">
+        <v>21</v>
+      </c>
+      <c r="C96" t="s">
+        <v>21</v>
+      </c>
+      <c r="D96" t="s">
+        <v>21</v>
+      </c>
+      <c r="E96" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" t="s">
+        <v>21</v>
+      </c>
+      <c r="G96" t="s">
+        <v>21</v>
+      </c>
+      <c r="H96" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>200</v>
+      </c>
+      <c r="B97" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" t="s">
+        <v>23</v>
+      </c>
+      <c r="D97" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" t="s">
+        <v>23</v>
+      </c>
+      <c r="G97" t="s">
+        <v>23</v>
+      </c>
+      <c r="H97" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>202</v>
+      </c>
+      <c r="B98" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" t="s">
+        <v>21</v>
+      </c>
+      <c r="E98" t="s">
+        <v>21</v>
+      </c>
+      <c r="F98" t="s">
+        <v>21</v>
+      </c>
+      <c r="G98" t="s">
+        <v>21</v>
+      </c>
+      <c r="H98" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>203</v>
+      </c>
+      <c r="B99" t="s">
+        <v>23</v>
+      </c>
+      <c r="C99" t="s">
+        <v>20</v>
+      </c>
+      <c r="D99" t="s">
+        <v>20</v>
+      </c>
+      <c r="E99" t="s">
+        <v>23</v>
+      </c>
+      <c r="F99" t="s">
+        <v>23</v>
+      </c>
+      <c r="G99" t="s">
+        <v>23</v>
+      </c>
+      <c r="H99" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>205</v>
+      </c>
+      <c r="B100" t="s">
+        <v>21</v>
+      </c>
+      <c r="C100" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" t="s">
+        <v>21</v>
+      </c>
+      <c r="G100" t="s">
+        <v>21</v>
+      </c>
+      <c r="H100" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>207</v>
+      </c>
+      <c r="B101" t="s">
+        <v>23</v>
+      </c>
+      <c r="C101" t="s">
+        <v>23</v>
+      </c>
+      <c r="D101" t="s">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" t="s">
+        <v>20</v>
+      </c>
+      <c r="G101" t="s">
+        <v>23</v>
+      </c>
+      <c r="H101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>209</v>
+      </c>
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+      <c r="C102" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" t="s">
+        <v>21</v>
+      </c>
+      <c r="E102" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" t="s">
+        <v>20</v>
+      </c>
+      <c r="G102" t="s">
+        <v>20</v>
+      </c>
+      <c r="H102" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>211</v>
+      </c>
+      <c r="B103" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" t="s">
+        <v>23</v>
+      </c>
+      <c r="D103" t="s">
+        <v>23</v>
+      </c>
+      <c r="E103" t="s">
+        <v>23</v>
+      </c>
+      <c r="F103" t="s">
+        <v>23</v>
+      </c>
+      <c r="G103" t="s">
+        <v>20</v>
+      </c>
+      <c r="H103" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>213</v>
+      </c>
+      <c r="B104" t="s">
+        <v>21</v>
+      </c>
+      <c r="C104" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" t="s">
+        <v>21</v>
+      </c>
+      <c r="E104" t="s">
+        <v>21</v>
+      </c>
+      <c r="F104" t="s">
+        <v>21</v>
+      </c>
+      <c r="G104" t="s">
+        <v>21</v>
+      </c>
+      <c r="H104" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>215</v>
+      </c>
+      <c r="B105" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" t="s">
+        <v>23</v>
+      </c>
+      <c r="D105" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" t="s">
+        <v>23</v>
+      </c>
+      <c r="F105" t="s">
+        <v>23</v>
+      </c>
+      <c r="G105" t="s">
+        <v>23</v>
+      </c>
+      <c r="H105" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>217</v>
+      </c>
+      <c r="B106" t="s">
+        <v>20</v>
+      </c>
+      <c r="C106" t="s">
+        <v>20</v>
+      </c>
+      <c r="D106" t="s">
+        <v>21</v>
+      </c>
+      <c r="E106" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106" t="s">
+        <v>21</v>
+      </c>
+      <c r="G106" t="s">
+        <v>21</v>
+      </c>
+      <c r="H106" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>218</v>
+      </c>
+      <c r="B107" t="s">
+        <v>23</v>
+      </c>
+      <c r="C107" t="s">
+        <v>20</v>
+      </c>
+      <c r="D107" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" t="s">
+        <v>23</v>
+      </c>
+      <c r="F107" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" t="s">
+        <v>23</v>
+      </c>
+      <c r="H107" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>220</v>
+      </c>
+      <c r="B108" t="s">
+        <v>21</v>
+      </c>
+      <c r="C108" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" t="s">
+        <v>20</v>
+      </c>
+      <c r="E108" t="s">
+        <v>20</v>
+      </c>
+      <c r="F108" t="s">
+        <v>21</v>
+      </c>
+      <c r="G108" t="s">
+        <v>21</v>
+      </c>
+      <c r="H108" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>222</v>
+      </c>
+      <c r="B109" t="s">
+        <v>23</v>
+      </c>
+      <c r="C109" t="s">
+        <v>23</v>
+      </c>
+      <c r="D109" t="s">
+        <v>23</v>
+      </c>
+      <c r="E109" t="s">
+        <v>20</v>
+      </c>
+      <c r="F109" t="s">
+        <v>20</v>
+      </c>
+      <c r="G109" t="s">
+        <v>23</v>
+      </c>
+      <c r="H109" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>224</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" t="s">
+        <v>21</v>
+      </c>
+      <c r="D110" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" t="s">
+        <v>21</v>
+      </c>
+      <c r="F110" t="s">
+        <v>20</v>
+      </c>
+      <c r="G110" t="s">
+        <v>20</v>
+      </c>
+      <c r="H110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>226</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" t="s">
+        <v>23</v>
+      </c>
+      <c r="D111" t="s">
+        <v>23</v>
+      </c>
+      <c r="E111" t="s">
+        <v>23</v>
+      </c>
+      <c r="F111" t="s">
+        <v>23</v>
+      </c>
+      <c r="G111" t="s">
+        <v>20</v>
+      </c>
+      <c r="H111" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>228</v>
+      </c>
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" t="s">
+        <v>21</v>
+      </c>
+      <c r="D112" t="s">
+        <v>21</v>
+      </c>
+      <c r="E112" t="s">
+        <v>21</v>
+      </c>
+      <c r="F112" t="s">
+        <v>21</v>
+      </c>
+      <c r="G112" t="s">
+        <v>21</v>
+      </c>
+      <c r="H112" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>230</v>
+      </c>
+      <c r="B113" t="s">
+        <v>23</v>
+      </c>
+      <c r="C113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D113" t="s">
+        <v>23</v>
+      </c>
+      <c r="E113" t="s">
+        <v>23</v>
+      </c>
+      <c r="F113" t="s">
+        <v>23</v>
+      </c>
+      <c r="G113" t="s">
+        <v>23</v>
+      </c>
+      <c r="H113" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>232</v>
+      </c>
+      <c r="B114" t="s">
+        <v>20</v>
+      </c>
+      <c r="C114" t="s">
+        <v>20</v>
+      </c>
+      <c r="D114" t="s">
+        <v>21</v>
+      </c>
+      <c r="E114" t="s">
+        <v>21</v>
+      </c>
+      <c r="F114" t="s">
+        <v>21</v>
+      </c>
+      <c r="G114" t="s">
+        <v>21</v>
+      </c>
+      <c r="H114" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>233</v>
+      </c>
+      <c r="B115" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" t="s">
+        <v>20</v>
+      </c>
+      <c r="D115" t="s">
+        <v>20</v>
+      </c>
+      <c r="E115" t="s">
+        <v>23</v>
+      </c>
+      <c r="F115" t="s">
+        <v>23</v>
+      </c>
+      <c r="G115" t="s">
+        <v>23</v>
+      </c>
+      <c r="H115" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>235</v>
+      </c>
+      <c r="B116" t="s">
+        <v>21</v>
+      </c>
+      <c r="C116" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" t="s">
+        <v>20</v>
+      </c>
+      <c r="E116" t="s">
+        <v>20</v>
+      </c>
+      <c r="F116" t="s">
+        <v>21</v>
+      </c>
+      <c r="G116" t="s">
+        <v>21</v>
+      </c>
+      <c r="H116" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>237</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" t="s">
+        <v>23</v>
+      </c>
+      <c r="D117" t="s">
+        <v>23</v>
+      </c>
+      <c r="E117" t="s">
+        <v>20</v>
+      </c>
+      <c r="F117" t="s">
+        <v>20</v>
+      </c>
+      <c r="G117" t="s">
+        <v>23</v>
+      </c>
+      <c r="H117" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>239</v>
+      </c>
+      <c r="B118" t="s">
+        <v>21</v>
+      </c>
+      <c r="C118" t="s">
+        <v>21</v>
+      </c>
+      <c r="D118" t="s">
+        <v>21</v>
+      </c>
+      <c r="E118" t="s">
+        <v>21</v>
+      </c>
+      <c r="F118" t="s">
+        <v>20</v>
+      </c>
+      <c r="G118" t="s">
+        <v>20</v>
+      </c>
+      <c r="H118" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>241</v>
+      </c>
+      <c r="B119" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119" t="s">
+        <v>23</v>
+      </c>
+      <c r="E119" t="s">
+        <v>23</v>
+      </c>
+      <c r="F119" t="s">
+        <v>23</v>
+      </c>
+      <c r="G119" t="s">
+        <v>20</v>
+      </c>
+      <c r="H119" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>243</v>
+      </c>
+      <c r="B120" t="s">
+        <v>21</v>
+      </c>
+      <c r="C120" t="s">
+        <v>21</v>
+      </c>
+      <c r="D120" t="s">
+        <v>21</v>
+      </c>
+      <c r="E120" t="s">
+        <v>21</v>
+      </c>
+      <c r="F120" t="s">
+        <v>21</v>
+      </c>
+      <c r="G120" t="s">
+        <v>21</v>
+      </c>
+      <c r="H120" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>245</v>
+      </c>
+      <c r="B121" t="s">
+        <v>23</v>
+      </c>
+      <c r="C121" t="s">
+        <v>23</v>
+      </c>
+      <c r="D121" t="s">
+        <v>23</v>
+      </c>
+      <c r="E121" t="s">
+        <v>23</v>
+      </c>
+      <c r="F121" t="s">
+        <v>23</v>
+      </c>
+      <c r="G121" t="s">
+        <v>23</v>
+      </c>
+      <c r="H121" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>247</v>
+      </c>
+      <c r="B122" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" t="s">
+        <v>20</v>
+      </c>
+      <c r="D122" t="s">
+        <v>21</v>
+      </c>
+      <c r="E122" t="s">
+        <v>21</v>
+      </c>
+      <c r="F122" t="s">
+        <v>21</v>
+      </c>
+      <c r="G122" t="s">
+        <v>21</v>
+      </c>
+      <c r="H122" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>248</v>
+      </c>
+      <c r="B123" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" t="s">
+        <v>20</v>
+      </c>
+      <c r="D123" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123" t="s">
+        <v>23</v>
+      </c>
+      <c r="F123" t="s">
+        <v>23</v>
+      </c>
+      <c r="G123" t="s">
+        <v>23</v>
+      </c>
+      <c r="H123" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>250</v>
+      </c>
+      <c r="B124" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" t="s">
+        <v>20</v>
+      </c>
+      <c r="E124" t="s">
+        <v>20</v>
+      </c>
+      <c r="F124" t="s">
+        <v>21</v>
+      </c>
+      <c r="G124" t="s">
+        <v>21</v>
+      </c>
+      <c r="H124" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>252</v>
+      </c>
+      <c r="B125" t="s">
+        <v>23</v>
+      </c>
+      <c r="C125" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" t="s">
+        <v>23</v>
+      </c>
+      <c r="E125" t="s">
+        <v>20</v>
+      </c>
+      <c r="F125" t="s">
+        <v>20</v>
+      </c>
+      <c r="G125" t="s">
+        <v>23</v>
+      </c>
+      <c r="H125" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>254</v>
+      </c>
+      <c r="B126" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126" t="s">
+        <v>21</v>
+      </c>
+      <c r="D126" t="s">
+        <v>21</v>
+      </c>
+      <c r="E126" t="s">
+        <v>21</v>
+      </c>
+      <c r="F126" t="s">
+        <v>20</v>
+      </c>
+      <c r="G126" t="s">
+        <v>20</v>
+      </c>
+      <c r="H126" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>256</v>
+      </c>
+      <c r="B127" t="s">
+        <v>23</v>
+      </c>
+      <c r="C127" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" t="s">
+        <v>23</v>
+      </c>
+      <c r="E127" t="s">
+        <v>23</v>
+      </c>
+      <c r="F127" t="s">
+        <v>23</v>
+      </c>
+      <c r="G127" t="s">
+        <v>20</v>
+      </c>
+      <c r="H127" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>258</v>
+      </c>
+      <c r="B128" t="s">
+        <v>21</v>
+      </c>
+      <c r="C128" t="s">
+        <v>21</v>
+      </c>
+      <c r="D128" t="s">
+        <v>21</v>
+      </c>
+      <c r="E128" t="s">
+        <v>21</v>
+      </c>
+      <c r="F128" t="s">
+        <v>21</v>
+      </c>
+      <c r="G128" t="s">
+        <v>21</v>
+      </c>
+      <c r="H128" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>260</v>
+      </c>
+      <c r="B129" t="s">
+        <v>23</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129" t="s">
+        <v>23</v>
+      </c>
+      <c r="E129" t="s">
+        <v>23</v>
+      </c>
+      <c r="F129" t="s">
+        <v>23</v>
+      </c>
+      <c r="G129" t="s">
+        <v>23</v>
+      </c>
+      <c r="H129" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>262</v>
+      </c>
+      <c r="B130" t="s">
+        <v>20</v>
+      </c>
+      <c r="C130" t="s">
+        <v>20</v>
+      </c>
+      <c r="D130" t="s">
+        <v>21</v>
+      </c>
+      <c r="E130" t="s">
+        <v>21</v>
+      </c>
+      <c r="F130" t="s">
+        <v>21</v>
+      </c>
+      <c r="G130" t="s">
+        <v>21</v>
+      </c>
+      <c r="H130" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>263</v>
+      </c>
+      <c r="B131" t="s">
+        <v>23</v>
+      </c>
+      <c r="C131" t="s">
+        <v>20</v>
+      </c>
+      <c r="D131" t="s">
+        <v>20</v>
+      </c>
+      <c r="E131" t="s">
+        <v>23</v>
+      </c>
+      <c r="F131" t="s">
+        <v>23</v>
+      </c>
+      <c r="G131" t="s">
+        <v>23</v>
+      </c>
+      <c r="H131" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" t="s">
+        <v>21</v>
+      </c>
+      <c r="C132" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" t="s">
+        <v>20</v>
+      </c>
+      <c r="E132" t="s">
+        <v>20</v>
+      </c>
+      <c r="F132" t="s">
+        <v>21</v>
+      </c>
+      <c r="G132" t="s">
+        <v>21</v>
+      </c>
+      <c r="H132" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>267</v>
+      </c>
+      <c r="B133" t="s">
+        <v>23</v>
+      </c>
+      <c r="C133" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133" t="s">
+        <v>23</v>
+      </c>
+      <c r="E133" t="s">
+        <v>20</v>
+      </c>
+      <c r="F133" t="s">
+        <v>20</v>
+      </c>
+      <c r="G133" t="s">
+        <v>23</v>
+      </c>
+      <c r="H133" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2254,6 +4848,798 @@
       </c>
       <c r="C51" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>151.0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>152.0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>153.0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>155.0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>156.0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>159.0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>160.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>161.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>162.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>136</v>
+      </c>
+      <c r="C63" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>163.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>164.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>166.0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>167.0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>168.0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>169.0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>170.0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>171.0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>172.0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>174.0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>175.0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>176.0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>162</v>
+      </c>
+      <c r="C77" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>177.0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>178.0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>166</v>
+      </c>
+      <c r="C79" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>179.0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>180.0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>170</v>
+      </c>
+      <c r="C81" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>182.0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>183.0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>184.0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>185.0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>186.0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>181</v>
+      </c>
+      <c r="C87" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>187.0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>183</v>
+      </c>
+      <c r="C88" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>188.0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>185</v>
+      </c>
+      <c r="C89" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>188</v>
+      </c>
+      <c r="C91" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>191.0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>190</v>
+      </c>
+      <c r="C92" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>192.0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>192</v>
+      </c>
+      <c r="C93" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>193.0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>194</v>
+      </c>
+      <c r="C94" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>194.0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>196</v>
+      </c>
+      <c r="C95" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>195.0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>198</v>
+      </c>
+      <c r="C96" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>196.0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>200</v>
+      </c>
+      <c r="C97" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>203</v>
+      </c>
+      <c r="C99" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>199.0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>207</v>
+      </c>
+      <c r="C101" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>201.0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>209</v>
+      </c>
+      <c r="C102" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>202.0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>211</v>
+      </c>
+      <c r="C103" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>203.0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>204.0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>215</v>
+      </c>
+      <c r="C105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>206.0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>218</v>
+      </c>
+      <c r="C107" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>207.0</v>
+      </c>
+      <c r="B108" t="s">
+        <v>220</v>
+      </c>
+      <c r="C108" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>208.0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>222</v>
+      </c>
+      <c r="C109" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>209.0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>224</v>
+      </c>
+      <c r="C110" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>210.0</v>
+      </c>
+      <c r="B111" t="s">
+        <v>226</v>
+      </c>
+      <c r="C111" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>211.0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>228</v>
+      </c>
+      <c r="C112" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>212.0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>230</v>
+      </c>
+      <c r="C113" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>214.0</v>
+      </c>
+      <c r="B115" t="s">
+        <v>233</v>
+      </c>
+      <c r="C115" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>215.0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>235</v>
+      </c>
+      <c r="C116" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>216.0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>237</v>
+      </c>
+      <c r="C117" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>217.0</v>
+      </c>
+      <c r="B118" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>218.0</v>
+      </c>
+      <c r="B119" t="s">
+        <v>241</v>
+      </c>
+      <c r="C119" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>219.0</v>
+      </c>
+      <c r="B120" t="s">
+        <v>243</v>
+      </c>
+      <c r="C120" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>220.0</v>
+      </c>
+      <c r="B121" t="s">
+        <v>245</v>
+      </c>
+      <c r="C121" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>222.0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>248</v>
+      </c>
+      <c r="C123" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>223.0</v>
+      </c>
+      <c r="B124" t="s">
+        <v>250</v>
+      </c>
+      <c r="C124" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>224.0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>252</v>
+      </c>
+      <c r="C125" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>225.0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>254</v>
+      </c>
+      <c r="C126" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>226.0</v>
+      </c>
+      <c r="B127" t="s">
+        <v>256</v>
+      </c>
+      <c r="C127" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>227.0</v>
+      </c>
+      <c r="B128" t="s">
+        <v>258</v>
+      </c>
+      <c r="C128" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>228.0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>260</v>
+      </c>
+      <c r="C129" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>230.0</v>
+      </c>
+      <c r="B131" t="s">
+        <v>263</v>
+      </c>
+      <c r="C131" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>231.0</v>
+      </c>
+      <c r="B132" t="s">
+        <v>265</v>
+      </c>
+      <c r="C132" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>232.0</v>
+      </c>
+      <c r="B133" t="s">
+        <v>267</v>
+      </c>
+      <c r="C133" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2354,6 +5740,88 @@
     <row r="49"/>
     <row r="50"/>
     <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated scheduling algorithm, Moving block mode, Javadocs, and GUI displays
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -67,148 +67,178 @@
     <t>Employee 1</t>
   </si>
   <si>
-    <t>6.00.00</t>
-  </si>
-  <si>
-    <t>7.180.0</t>
-  </si>
-  <si>
-    <t>7.210.0</t>
-  </si>
-  <si>
-    <t>7.450.0</t>
-  </si>
-  <si>
-    <t>14.00.00</t>
+    <t>06.10.00</t>
   </si>
   <si>
     <t>Employee 2</t>
   </si>
   <si>
-    <t>06.00.00</t>
+    <t>6.25.0</t>
   </si>
   <si>
     <t>Employee 3</t>
   </si>
   <si>
-    <t>2.7.0</t>
+    <t>6.40.0</t>
   </si>
   <si>
     <t>Employee 4</t>
   </si>
   <si>
-    <t>6.7.0</t>
+    <t>6.55.0</t>
   </si>
   <si>
     <t>Employee 5</t>
   </si>
   <si>
-    <t>2.14.0</t>
+    <t>7.10.0</t>
   </si>
   <si>
     <t>Employee 6</t>
   </si>
   <si>
-    <t>6.14.0</t>
+    <t>7.25.0</t>
+  </si>
+  <si>
+    <t>Employee 7</t>
+  </si>
+  <si>
+    <t>7.40.0</t>
+  </si>
+  <si>
+    <t>PIONEER</t>
+  </si>
+  <si>
+    <t>EDGEBROOK</t>
+  </si>
+  <si>
+    <t>PITT</t>
+  </si>
+  <si>
+    <t>WHITED</t>
+  </si>
+  <si>
+    <t>SOUTH BANK</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>INGLEWOOD</t>
+  </si>
+  <si>
+    <t>OVERBROOK</t>
+  </si>
+  <si>
+    <t>GLENBURY</t>
+  </si>
+  <si>
+    <t>DORMONT</t>
+  </si>
+  <si>
+    <t>MT LEBANON</t>
+  </si>
+  <si>
+    <t>POPLAR</t>
+  </si>
+  <si>
+    <t>CASTLE SHANON</t>
+  </si>
+  <si>
+    <t>GLEBURY</t>
+  </si>
+  <si>
+    <t>Employee 9</t>
+  </si>
+  <si>
+    <t>Employee 10</t>
+  </si>
+  <si>
+    <t>Employee 11</t>
+  </si>
+  <si>
+    <t>Employee 12</t>
+  </si>
+  <si>
+    <t>Employee 13</t>
+  </si>
+  <si>
+    <t>Employee 14</t>
+  </si>
+  <si>
+    <t>Employee 15</t>
+  </si>
+  <si>
+    <t>6:10am</t>
+  </si>
+  <si>
+    <t>10:10am</t>
+  </si>
+  <si>
+    <t>10:40am</t>
+  </si>
+  <si>
+    <t>2:40pm</t>
+  </si>
+  <si>
+    <t>6:25am</t>
+  </si>
+  <si>
+    <t>10:25am</t>
+  </si>
+  <si>
+    <t>10:55am</t>
+  </si>
+  <si>
+    <t>2:55pm</t>
+  </si>
+  <si>
+    <t>6:40am</t>
+  </si>
+  <si>
+    <t>11:10am</t>
+  </si>
+  <si>
+    <t>3:10am</t>
   </si>
   <si>
     <t>Employee 8</t>
   </si>
   <si>
-    <t>6:10am</t>
-  </si>
-  <si>
-    <t>10:10am</t>
-  </si>
-  <si>
-    <t>10:40am</t>
-  </si>
-  <si>
-    <t>2:40pm</t>
-  </si>
-  <si>
-    <t>2.21.0</t>
-  </si>
-  <si>
-    <t>Employee 9</t>
-  </si>
-  <si>
-    <t>6:20am</t>
-  </si>
-  <si>
-    <t>10:20am</t>
-  </si>
-  <si>
-    <t>10:50am</t>
-  </si>
-  <si>
-    <t>2:50pm</t>
-  </si>
-  <si>
-    <t>6.21.0</t>
-  </si>
-  <si>
-    <t>Employee 10</t>
-  </si>
-  <si>
-    <t>6:30am</t>
-  </si>
-  <si>
-    <t>10:30am</t>
-  </si>
-  <si>
-    <t>10:60am</t>
-  </si>
-  <si>
-    <t>2:60pm</t>
-  </si>
-  <si>
-    <t>2.28.0</t>
-  </si>
-  <si>
-    <t>Employee 11</t>
-  </si>
-  <si>
-    <t>6:40am</t>
-  </si>
-  <si>
-    <t>11:10am</t>
-  </si>
-  <si>
-    <t>3:10am</t>
-  </si>
-  <si>
-    <t>6.28.0</t>
-  </si>
-  <si>
-    <t>Employee 12</t>
-  </si>
-  <si>
-    <t>6:50am</t>
-  </si>
-  <si>
-    <t>11:20am</t>
-  </si>
-  <si>
-    <t>3:20am</t>
-  </si>
-  <si>
-    <t>2.35.0</t>
-  </si>
-  <si>
-    <t>Employee 13</t>
-  </si>
-  <si>
-    <t>6:60am</t>
-  </si>
-  <si>
-    <t>11:30am</t>
-  </si>
-  <si>
-    <t>3:30am</t>
-  </si>
-  <si>
-    <t>6.35.0</t>
+    <t>6:55am</t>
+  </si>
+  <si>
+    <t>11:25am</t>
+  </si>
+  <si>
+    <t>3:25am</t>
+  </si>
+  <si>
+    <t>7:10am</t>
+  </si>
+  <si>
+    <t>11:40am</t>
+  </si>
+  <si>
+    <t>3:40am</t>
+  </si>
+  <si>
+    <t>7:25am</t>
+  </si>
+  <si>
+    <t>11:55am</t>
+  </si>
+  <si>
+    <t>3:55am</t>
+  </si>
+  <si>
+    <t>7:40am</t>
+  </si>
+  <si>
+    <t>12:10am</t>
+  </si>
+  <si>
+    <t>4:10am</t>
   </si>
 </sst>
 </file>
@@ -261,121 +291,240 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -428,68 +577,79 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>101.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>102.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>103.0</v>
+        <v>5.0</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>104.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>105.0</v>
+        <v>9.0</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>106.0</v>
+        <v>11.0</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -516,94 +676,135 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>108.0</v>
+        <v>3.0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>109.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>110.0</v>
+        <v>7.0</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>111.0</v>
+        <v>9.0</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>112.0</v>
+        <v>11.0</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>113.0</v>
+        <v>13.0</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Throwing ConcurrentModificationException in TrainSystem
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -94,105 +94,90 @@
     <t>7.10.0</t>
   </si>
   <si>
+    <t>PIONEER</t>
+  </si>
+  <si>
+    <t>EDGEBROOK</t>
+  </si>
+  <si>
+    <t>PITT</t>
+  </si>
+  <si>
+    <t>WHITED</t>
+  </si>
+  <si>
+    <t>SOUTH BANK</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>INGLEWOOD</t>
+  </si>
+  <si>
+    <t>OVERBROOK</t>
+  </si>
+  <si>
+    <t>GLENBURY</t>
+  </si>
+  <si>
+    <t>DORMONT</t>
+  </si>
+  <si>
+    <t>MT LEBANON</t>
+  </si>
+  <si>
+    <t>POPLAR</t>
+  </si>
+  <si>
+    <t>CASTLE SHANON</t>
+  </si>
+  <si>
+    <t>GLEBURY</t>
+  </si>
+  <si>
+    <t>Employee 7</t>
+  </si>
+  <si>
+    <t>Employee 8</t>
+  </si>
+  <si>
+    <t>Employee 9</t>
+  </si>
+  <si>
+    <t>Employee 10</t>
+  </si>
+  <si>
+    <t>Employee 11</t>
+  </si>
+  <si>
+    <t>6:10am</t>
+  </si>
+  <si>
+    <t>10:10am</t>
+  </si>
+  <si>
+    <t>10:40am</t>
+  </si>
+  <si>
+    <t>2:40pm</t>
+  </si>
+  <si>
+    <t>6:25am</t>
+  </si>
+  <si>
+    <t>10:25am</t>
+  </si>
+  <si>
+    <t>10:55am</t>
+  </si>
+  <si>
+    <t>2:55pm</t>
+  </si>
+  <si>
     <t>Employee 6</t>
   </si>
   <si>
-    <t>7.25.0</t>
-  </si>
-  <si>
-    <t>Employee 7</t>
-  </si>
-  <si>
-    <t>7.40.0</t>
-  </si>
-  <si>
-    <t>PIONEER</t>
-  </si>
-  <si>
-    <t>EDGEBROOK</t>
-  </si>
-  <si>
-    <t>PITT</t>
-  </si>
-  <si>
-    <t>WHITED</t>
-  </si>
-  <si>
-    <t>SOUTH BANK</t>
-  </si>
-  <si>
-    <t>CENTRAL</t>
-  </si>
-  <si>
-    <t>INGLEWOOD</t>
-  </si>
-  <si>
-    <t>OVERBROOK</t>
-  </si>
-  <si>
-    <t>GLENBURY</t>
-  </si>
-  <si>
-    <t>DORMONT</t>
-  </si>
-  <si>
-    <t>MT LEBANON</t>
-  </si>
-  <si>
-    <t>POPLAR</t>
-  </si>
-  <si>
-    <t>CASTLE SHANON</t>
-  </si>
-  <si>
-    <t>GLEBURY</t>
-  </si>
-  <si>
-    <t>Employee 9</t>
-  </si>
-  <si>
-    <t>Employee 10</t>
-  </si>
-  <si>
-    <t>Employee 11</t>
-  </si>
-  <si>
-    <t>Employee 12</t>
-  </si>
-  <si>
-    <t>Employee 13</t>
-  </si>
-  <si>
-    <t>Employee 14</t>
-  </si>
-  <si>
-    <t>Employee 15</t>
-  </si>
-  <si>
-    <t>6:10am</t>
-  </si>
-  <si>
-    <t>10:10am</t>
-  </si>
-  <si>
-    <t>10:40am</t>
-  </si>
-  <si>
-    <t>2:40pm</t>
-  </si>
-  <si>
-    <t>6:25am</t>
-  </si>
-  <si>
-    <t>10:25am</t>
-  </si>
-  <si>
-    <t>10:55am</t>
-  </si>
-  <si>
-    <t>2:55pm</t>
-  </si>
-  <si>
     <t>6:40am</t>
   </si>
   <si>
@@ -202,9 +187,6 @@
     <t>3:10am</t>
   </si>
   <si>
-    <t>Employee 8</t>
-  </si>
-  <si>
     <t>6:55am</t>
   </si>
   <si>
@@ -221,24 +203,6 @@
   </si>
   <si>
     <t>3:40am</t>
-  </si>
-  <si>
-    <t>7:25am</t>
-  </si>
-  <si>
-    <t>11:55am</t>
-  </si>
-  <si>
-    <t>3:55am</t>
-  </si>
-  <si>
-    <t>7:40am</t>
-  </si>
-  <si>
-    <t>12:10am</t>
-  </si>
-  <si>
-    <t>4:10am</t>
   </si>
 </sst>
 </file>
@@ -294,16 +258,16 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2">
@@ -311,16 +275,16 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
@@ -328,16 +292,16 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -345,16 +309,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -362,169 +326,101 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -630,28 +526,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -676,58 +550,58 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>36</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>43</v>
-      </c>
       <c r="S1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="T1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="U1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +609,7 @@
         <v>3.0</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -746,7 +620,7 @@
         <v>5.0</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -757,7 +631,7 @@
         <v>7.0</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -768,7 +642,7 @@
         <v>9.0</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -779,32 +653,10 @@
         <v>11.0</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Train ID bug fixed
</commit_message>
<xml_diff>
--- a/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
+++ b/TrainSystem/src/com/rogueone/assets/altSchedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -82,87 +82,72 @@
     <t>6.40.0</t>
   </si>
   <si>
+    <t>PIONEER</t>
+  </si>
+  <si>
+    <t>EDGEBROOK</t>
+  </si>
+  <si>
+    <t>PITT</t>
+  </si>
+  <si>
+    <t>WHITED</t>
+  </si>
+  <si>
+    <t>SOUTH BANK</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>INGLEWOOD</t>
+  </si>
+  <si>
+    <t>OVERBROOK</t>
+  </si>
+  <si>
+    <t>GLENBURY</t>
+  </si>
+  <si>
+    <t>DORMONT</t>
+  </si>
+  <si>
+    <t>MT LEBANON</t>
+  </si>
+  <si>
+    <t>POPLAR</t>
+  </si>
+  <si>
+    <t>CASTLE SHANON</t>
+  </si>
+  <si>
+    <t>GLEBURY</t>
+  </si>
+  <si>
+    <t>Employee 5</t>
+  </si>
+  <si>
+    <t>Employee 6</t>
+  </si>
+  <si>
+    <t>Employee 7</t>
+  </si>
+  <si>
+    <t>6:10am</t>
+  </si>
+  <si>
+    <t>10:10am</t>
+  </si>
+  <si>
+    <t>10:40am</t>
+  </si>
+  <si>
+    <t>2:40pm</t>
+  </si>
+  <si>
     <t>Employee 4</t>
   </si>
   <si>
-    <t>6.55.0</t>
-  </si>
-  <si>
-    <t>Employee 5</t>
-  </si>
-  <si>
-    <t>7.10.0</t>
-  </si>
-  <si>
-    <t>PIONEER</t>
-  </si>
-  <si>
-    <t>EDGEBROOK</t>
-  </si>
-  <si>
-    <t>PITT</t>
-  </si>
-  <si>
-    <t>WHITED</t>
-  </si>
-  <si>
-    <t>SOUTH BANK</t>
-  </si>
-  <si>
-    <t>CENTRAL</t>
-  </si>
-  <si>
-    <t>INGLEWOOD</t>
-  </si>
-  <si>
-    <t>OVERBROOK</t>
-  </si>
-  <si>
-    <t>GLENBURY</t>
-  </si>
-  <si>
-    <t>DORMONT</t>
-  </si>
-  <si>
-    <t>MT LEBANON</t>
-  </si>
-  <si>
-    <t>POPLAR</t>
-  </si>
-  <si>
-    <t>CASTLE SHANON</t>
-  </si>
-  <si>
-    <t>GLEBURY</t>
-  </si>
-  <si>
-    <t>Employee 7</t>
-  </si>
-  <si>
-    <t>Employee 8</t>
-  </si>
-  <si>
-    <t>Employee 9</t>
-  </si>
-  <si>
-    <t>Employee 10</t>
-  </si>
-  <si>
-    <t>Employee 11</t>
-  </si>
-  <si>
-    <t>6:10am</t>
-  </si>
-  <si>
-    <t>10:10am</t>
-  </si>
-  <si>
-    <t>10:40am</t>
-  </si>
-  <si>
-    <t>2:40pm</t>
-  </si>
-  <si>
     <t>6:25am</t>
   </si>
   <si>
@@ -175,9 +160,6 @@
     <t>2:55pm</t>
   </si>
   <si>
-    <t>Employee 6</t>
-  </si>
-  <si>
     <t>6:40am</t>
   </si>
   <si>
@@ -185,24 +167,6 @@
   </si>
   <si>
     <t>3:10am</t>
-  </si>
-  <si>
-    <t>6:55am</t>
-  </si>
-  <si>
-    <t>11:25am</t>
-  </si>
-  <si>
-    <t>3:25am</t>
-  </si>
-  <si>
-    <t>7:10am</t>
-  </si>
-  <si>
-    <t>11:40am</t>
-  </si>
-  <si>
-    <t>3:40am</t>
   </si>
 </sst>
 </file>
@@ -258,16 +222,16 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -275,16 +239,16 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -292,135 +256,67 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +369,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="B2" t="s">
         <v>16</v>
@@ -484,7 +380,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -495,35 +391,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -550,66 +424,66 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>32</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R1" t="s">
-        <v>39</v>
-      </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="U1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -617,10 +491,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -628,35 +502,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>